<commit_message>
Tested with tck-dmn text conformance kit
</commit_message>
<xml_diff>
--- a/DMNexamples/ExampleExecuteInterest1.xlsx
+++ b/DMNexamples/ExampleExecuteInterest1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82cfe7acc6d68563/Documents/PyPI/github/pyDMNrules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82cfe7acc6d68563/Documents/PyPI/github/DecisionCentral/DMNexamples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{8B258FCF-2450-4C0B-9D20-F4F0B2EB6BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2AD805E-5078-4655-905B-8352BE55B7AB}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="13_ncr:1_{8B258FCF-2450-4C0B-9D20-F4F0B2EB6BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EE337A2-6A36-49F4-AD8D-CB5ACE3094DD}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{028A0587-4E61-4813-9665-FF16B2928183}"/>
+    <workbookView xWindow="28680" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{028A0587-4E61-4813-9665-FF16B2928183}"/>
   </bookViews>
   <sheets>
     <sheet name="Decision" sheetId="2" r:id="rId1"/>
@@ -171,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -279,6 +279,15 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -327,14 +336,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -666,10 +675,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="2:3" ht="24.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="1" t="s">
@@ -700,7 +709,7 @@
   <dimension ref="B2:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F17" sqref="F17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -716,11 +725,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="4" t="s">
@@ -790,6 +799,9 @@
       <c r="H5" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>